<commit_message>
Added new code for 24 core on all Tested with 1,2,4,6,12,16,20,24 cores Added New graph to Excell file
</commit_message>
<xml_diff>
--- a/Uporedjivanje.xlsx
+++ b/Uporedjivanje.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pitch\OneDrive\Desktop\paralel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377775DB-CCA1-495D-BF32-1296E65C1BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6906370-54C5-473D-87FF-987B52312A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Cores</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Segments</t>
   </si>
 </sst>
 </file>
@@ -99,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +115,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +620,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$29</c:f>
+              <c:f>Sheet1!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -639,7 +643,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$29:$I$29</c:f>
+              <c:f>Sheet1!$B$30:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -682,7 +686,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$30</c:f>
+              <c:f>Sheet1!$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -705,7 +709,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$I$30</c:f>
+              <c:f>Sheet1!$B$31:$I$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -938,6 +942,413 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Total Time Same Segment</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Count</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD04-439A-8E36-3FD9CFC4B096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$I$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.02069091796875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83063530921936002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.597750663757324</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55203914642333896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57165861129760698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69061493873596103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.926050424575805</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1652591228485101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD04-439A-8E36-3FD9CFC4B096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1477112383"/>
+        <c:axId val="1467257119"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1477112383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1467257119"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1467257119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1477112383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1018,6 +1429,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2050,20 +2501,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>163512</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>577851</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>134938</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>368301</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2090,16 +3057,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>387349</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>454026</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2119,6 +3086,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9332B5DE-3C22-3D50-11AE-372B3380B8C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2390,10 +3393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="U13" sqref="U12:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2883,61 +3886,177 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>2</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="3">
         <v>4</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>6</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
         <v>12</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="3">
         <v>16</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <v>20</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2">
+        <v>6</v>
+      </c>
+      <c r="F30" s="2">
+        <v>12</v>
+      </c>
+      <c r="G30" s="2">
+        <v>16</v>
+      </c>
+      <c r="H30" s="2">
+        <v>20</v>
+      </c>
+      <c r="I30" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B31" s="4">
         <v>0.79065847396850497</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C31" s="4">
         <v>0.83271574974060003</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <v>0.57837820053100497</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E31" s="4">
         <v>0.67824387550354004</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F31" s="4">
         <v>0.74315524101257302</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G31" s="4">
         <v>0.63578677177429199</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H31" s="4">
         <v>0.58605408668518</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I31" s="4">
         <v>0.73266506195068304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3">
+        <v>24</v>
+      </c>
+      <c r="C36" s="3">
+        <v>24</v>
+      </c>
+      <c r="D36" s="3">
+        <v>24</v>
+      </c>
+      <c r="E36" s="3">
+        <v>24</v>
+      </c>
+      <c r="F36" s="3">
+        <v>24</v>
+      </c>
+      <c r="G36" s="3">
+        <v>24</v>
+      </c>
+      <c r="H36" s="3">
+        <v>24</v>
+      </c>
+      <c r="I36" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2">
+        <v>6</v>
+      </c>
+      <c r="F37" s="2">
+        <v>12</v>
+      </c>
+      <c r="G37" s="2">
+        <v>16</v>
+      </c>
+      <c r="H37" s="2">
+        <v>20</v>
+      </c>
+      <c r="I37" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1.02069091796875</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.83063530921936002</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.597750663757324</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.55203914642333896</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0.57165861129760698</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0.69061493873596103</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.926050424575805</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1.1652591228485101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>